<commit_message>
added an observable collection to bind to listview
</commit_message>
<xml_diff>
--- a/ImportMultipleFormatFiles/FileFormatSpecifierUnicodeASCII.xlsx
+++ b/ImportMultipleFormatFiles/FileFormatSpecifierUnicodeASCII.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yinon\source\repos\Projects\dmr\Future Versions Macros\ImportMultipleFormatFiles\ImportMultipleFormatFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{1A9B9D70-1294-45B9-BB08-5089062CE654}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CCE291-66FF-4E92-B41E-DD1117491F66}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,11 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added an import definition button and bind its visibility to the file format chosen
</commit_message>
<xml_diff>
--- a/ImportMultipleFormatFiles/FileFormatSpecifierUnicodeASCII.xlsx
+++ b/ImportMultipleFormatFiles/FileFormatSpecifierUnicodeASCII.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yinon\source\repos\Projects\dmr\Future Versions Macros\ImportMultipleFormatFiles\ImportMultipleFormatFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CCE291-66FF-4E92-B41E-DD1117491F66}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AE9455-2DD0-471F-91A3-50138399CDE4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>FORMAT</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>xsd , xrdf</t>
+  </si>
+  <si>
+    <t>jpm</t>
+  </si>
+  <si>
+    <t>fdf</t>
+  </si>
+  <si>
+    <t>rdm</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>jpm but for ascii</t>
   </si>
 </sst>
 </file>
@@ -439,7 +454,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +486,9 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -482,6 +500,9 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -493,6 +514,9 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -504,6 +528,9 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -512,6 +539,12 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -520,6 +553,12 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -527,6 +566,12 @@
       </c>
       <c r="B8" t="s">
         <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>